<commit_message>
my_api/algorithm mixed;1st phase transition
</commit_message>
<xml_diff>
--- a/监控数据查看地址以及IMEI号.xlsx
+++ b/监控数据查看地址以及IMEI号.xlsx
@@ -480,6 +480,7 @@
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -587,8 +588,8 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>